<commit_message>
Added/removed data files for testing
</commit_message>
<xml_diff>
--- a/DataFiles/REMS2020_ExampleA_3_Data.xlsx
+++ b/DataFiles/REMS2020_ExampleA_3_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqmstow1\Documents\REMS - Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqmstow1\Documents\GitHub\REMS2020\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
     <sheet name="SoilLayerDatas" sheetId="7" r:id="rId5"/>
     <sheet name="Stats" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="92512" iterate="1" iterateCount="1"/>
+  <calcPr calcId="92512"/>
 </workbook>
 </file>
 
@@ -697,7 +697,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -732,39 +732,21 @@
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3">
-        <v>3</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -51131,7 +51113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1075"/>
   <sheetViews>
-    <sheetView topLeftCell="A1025" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A1075"/>
     </sheetView>
   </sheetViews>

</xml_diff>